<commit_message>
função máximo e mínimo
</commit_message>
<xml_diff>
--- a/conceito_funcoes.xlsx
+++ b/conceito_funcoes.xlsx
@@ -380,7 +380,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -470,17 +470,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -741,7 +730,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -768,103 +757,106 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+      <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -1175,13 +1167,13 @@
       <c r="C4" s="7">
         <v>872</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -1256,13 +1248,13 @@
       <c r="C10" s="7">
         <v>1190</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
       <c r="K10" s="5"/>
       <c r="L10" s="11">
         <f>COUNT(C4:C18)</f>
@@ -1693,7 +1685,7 @@
   <dimension ref="B5:R22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,309 +1700,309 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="52"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="45"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="40"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="39" t="s">
+      <c r="E7" s="31"/>
+      <c r="F7" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="39" t="s">
+      <c r="G7" s="26"/>
+      <c r="H7" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="41" t="s">
+      <c r="I7" s="20"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="M7" s="58"/>
+      <c r="M7" s="41"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="39" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="39" t="s">
+      <c r="E8" s="28"/>
+      <c r="F8" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="39" t="s">
+      <c r="I8" s="28"/>
+      <c r="J8" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="41" t="s">
+      <c r="K8" s="25"/>
+      <c r="L8" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="59"/>
-      <c r="O8" s="46" t="s">
+      <c r="M8" s="42"/>
+      <c r="O8" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="48"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="55"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="39" t="s">
+      <c r="G9" s="27"/>
+      <c r="H9" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="39" t="s">
+      <c r="I9" s="29"/>
+      <c r="J9" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="K9" s="30"/>
-      <c r="L9" s="41" t="s">
+      <c r="K9" s="25"/>
+      <c r="L9" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="M9" s="59"/>
-      <c r="O9" s="49"/>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="51"/>
+      <c r="M9" s="42"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="57"/>
+      <c r="Q9" s="57"/>
+      <c r="R9" s="58"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="39" t="s">
+      <c r="E10" s="28"/>
+      <c r="F10" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="39" t="s">
+      <c r="I10" s="28"/>
+      <c r="J10" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="K10" s="30"/>
-      <c r="L10" s="41" t="s">
+      <c r="K10" s="25"/>
+      <c r="L10" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="M10" s="59"/>
-      <c r="O10" s="49"/>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="51"/>
+      <c r="M10" s="42"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="57"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="58"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="39" t="s">
+      <c r="D11" s="34"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="K11" s="38" t="s">
+      <c r="K11" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="41" t="s">
+      <c r="L11" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="M11" s="60" t="s">
+      <c r="M11" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="O11" s="49"/>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="50"/>
-      <c r="R11" s="51"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="58"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="39" t="s">
+      <c r="C12" s="28"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="K12" s="31"/>
-      <c r="L12" s="41" t="s">
+      <c r="K12" s="26"/>
+      <c r="L12" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="M12" s="59"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="54"/>
+      <c r="M12" s="42"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="61"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="59"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="42"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="39" t="s">
+      <c r="B14" s="34"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="59"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="42"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="39" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="39" t="s">
+      <c r="E15" s="28"/>
+      <c r="F15" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="59"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="42"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="39" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="39" t="s">
+      <c r="E16" s="20"/>
+      <c r="F16" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="59"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="42"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="40"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="40" t="s">
+      <c r="B17" s="35"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="62" t="s">
+      <c r="G17" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="63"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="64"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="47"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="27">
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="62">
         <f>COUNTA(C7:C17,E7:E17,G7:G17,I7:I17,K7:K17,M7:M17)</f>
         <v>10</v>
       </c>
@@ -2019,22 +2011,28 @@
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="28"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="63">
+        <f>F22-F20</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="29"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="63">
+        <f>COUNTA(B7:B17,D7:D17,F7:F17,H7:H17,J7:J17,L7:L17)</f>
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>